<commit_message>
finalize with sending to outlook email local
</commit_message>
<xml_diff>
--- a/03-excel_password/test_excel_password.xlsx
+++ b/03-excel_password/test_excel_password.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22641b00c1421f6a/Documents/Personals/08-Portfolios/03-excel_password/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8000_{EF8881AC-DDD8-4FA8-8C5B-DC00CB63FF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="10_ncr:8000_{EF8881AC-DDD8-4FA8-8C5B-DC00CB63FF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75429FB4-8AA8-485B-A37F-9C9DF97AF9C8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CCC38A44-8C3F-417F-8D0A-C399DBE989BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>test123</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>test146</t>
+  </si>
+  <si>
+    <t>kolom</t>
   </si>
 </sst>
 </file>
@@ -166,6 +169,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,131 +492,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0284BDB6-6E95-4434-86E6-AB594D492825}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>